<commit_message>
Test more shared formulas
</commit_message>
<xml_diff>
--- a/tests/testthat/formulas.xlsx
+++ b/tests/testthat/formulas.xlsx
@@ -347,9 +347,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -359,11 +361,39 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <f t="shared" ref="B1:D1" si="0">N($A2)</f>
+        <f t="shared" ref="B1:C1" si="0">N($A2)</f>
         <v>0</v>
       </c>
       <c r="C1">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f>"Hello, ""World""!"</f>
+        <v>Hello, "World"!</v>
+      </c>
+      <c r="B2" t="str">
+        <f t="shared" ref="B2:C2" si="1">"Hello, ""World""!"</f>
+        <v>Hello, "World"!</v>
+      </c>
+      <c r="C2" t="str">
+        <f t="shared" si="1"/>
+        <v>Hello, "World"!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>MIN($D$2:$D$3)</f>
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:C3" si="2">MIN($D$2:$D$3)</f>
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Recognise operators in grouped formulas (fixes 26)
Before, it treated `-F10` as "not a reference" because it saw it as a single
entity, rather than the combination of an operator `-` and a reference `F10`.
This fixes it by treating operators as separators, so that it expects `-`, `*`
et al to be followed by a separate entity.
</commit_message>
<xml_diff>
--- a/tests/testthat/formulas.xlsx
+++ b/tests/testthat/formulas.xlsx
@@ -347,11 +347,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -397,6 +395,20 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>E4*F4</f>
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ref="B4:C4" si="3">F4*G4</f>
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Recognise operators in grouped formulas (fixes 26) (#27)
Before, it treated `-F10` as "not a reference" because it saw it as a single
entity, rather than the combination of an operator `-` and a reference `F10`.
This fixes it by treating operators as separators, so that it expects `-`, `*`
et al to be followed by a separate entity.
</commit_message>
<xml_diff>
--- a/tests/testthat/formulas.xlsx
+++ b/tests/testthat/formulas.xlsx
@@ -347,11 +347,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -397,6 +395,20 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>E4*F4</f>
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ref="B4:C4" si="3">F4*G4</f>
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>